<commit_message>
next step--welded and flash
</commit_message>
<xml_diff>
--- a/JLINK_OB_072/PCB/JLINK_OB_072/Project Outputs for JLINK_OB_072/JLINK_OB_072.xlsx
+++ b/JLINK_OB_072/PCB/JLINK_OB_072/Project Outputs for JLINK_OB_072/JLINK_OB_072.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
   <si>
     <t>Comment</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>2.54排针6p</t>
+  </si>
+  <si>
+    <t>[NoValue], *1</t>
   </si>
   <si>
     <t>HDR2.54-WS-6P</t>
@@ -578,8 +581,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" baseColWidth="0"/>
   <cols>
-    <col min="1" max="6" width="20.2109375" customWidth="1"/>
-    <col min="7" max="7" width="16.9609375" customWidth="1"/>
+    <col min="1" max="6" width="20.0546875" customWidth="1"/>
+    <col min="7" max="7" width="16.8046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -612,102 +615,104 @@
       <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="20" t="s">
+        <v>9</v>
+      </c>
       <c r="D2" s="20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="17">
         <v>4</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="17">
         <v>1</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="17">
         <v>1</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" s="17">
         <v>1</v>
@@ -716,19 +721,19 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="17">
         <v>1</v>
@@ -737,19 +742,19 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8" s="17">
         <v>1</v>
@@ -758,19 +763,17 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B9" s="16"/>
       <c r="C9" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F9" s="17">
         <v>1</v>
@@ -779,134 +782,134 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F10" s="17">
         <v>2</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F11" s="17">
         <v>4</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F12" s="17">
         <v>2</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F13" s="17">
         <v>2</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="29" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F14" s="17">
         <v>2</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F15" s="17">
         <v>1</v>
@@ -915,19 +918,19 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F16" s="17">
         <v>1</v>
@@ -936,19 +939,19 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F17" s="17">
         <v>1</v>

</xml_diff>